<commit_message>
Generate v2.0 draft outputs
</commit_message>
<xml_diff>
--- a/Controller/Outputs/PixelClockController_v2_0_BOM.xlsx
+++ b/Controller/Outputs/PixelClockController_v2_0_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\PCB Design\RGB Clock\PixelClockPCB\Controller\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3AE7D34-EEA8-4E6F-8466-087711BA1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D42AA63D-C2AA-40C3-82F9-C62C7A74B9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1155" windowWidth="18900" windowHeight="11055" xr2:uid="{30847BA0-5CB3-4C6F-8CE2-685864D78C23}"/>
+    <workbookView xWindow="1155" yWindow="1155" windowWidth="18900" windowHeight="11055" xr2:uid="{B8D26753-1C9F-4536-BE8D-B1EB6808D39B}"/>
   </bookViews>
   <sheets>
     <sheet name="PixelClockController_v2_0_BOM" sheetId="1" r:id="rId1"/>
@@ -846,7 +846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2811BB-3C32-460D-8F63-D2DF9D2BA3B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA215A3-4D0B-48A3-BEC1-D8D0D47E1F55}">
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>